<commit_message>
HP updated weekly content
</commit_message>
<xml_diff>
--- a/CourseStructrure_AY2023-24.xlsx
+++ b/CourseStructrure_AY2023-24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hp12384/Library/Mobile Documents/com~apple~CloudDocs/Documents/Teaching/UoB/Intro_to_Programming /EMAT10007-2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/hp12384_bristol_ac_uk/Documents/Teaching/UoB/EMAT10007_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94D3B256-24FF-4E4F-8D7C-06948EE92458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{94D3B256-24FF-4E4F-8D7C-06948EE92458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D7434F7-070F-D145-9855-37B91F6CA1C2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{EB69D0A4-597B-4DBB-A11D-3E8D6AA8DFB6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -59,24 +59,12 @@
     <t>Programming Fundamentals</t>
   </si>
   <si>
-    <t>Variables &amp; Operators</t>
-  </si>
-  <si>
-    <t>Control flow</t>
-  </si>
-  <si>
-    <t>Loops</t>
-  </si>
-  <si>
     <t>Data Structures (Lists)</t>
   </si>
   <si>
     <t>Working with data</t>
   </si>
   <si>
-    <t>Reading data, Matplotlib</t>
-  </si>
-  <si>
     <t>Writing code that works</t>
   </si>
   <si>
@@ -150,6 +138,24 @@
   </si>
   <si>
     <t>2022/23 structure for reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coursework support session </t>
+  </si>
+  <si>
+    <t>Objects, Variables &amp; Operators</t>
+  </si>
+  <si>
+    <t>Control Structures: Conditional Statements</t>
+  </si>
+  <si>
+    <t>Control Structures: Loops</t>
+  </si>
+  <si>
+    <t>Reading and plotting data, Matplotlib</t>
+  </si>
+  <si>
+    <t>CW set</t>
   </si>
 </sst>
 </file>
@@ -349,12 +355,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -364,16 +364,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -690,23 +698,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9138578E-7460-4A95-82D6-FE3AF5733998}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="105.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -723,79 +731,74 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -804,160 +807,157 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9" s="10"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>13</v>
+      <c r="C12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="18">
+      <c r="C13" s="17"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="15">
         <v>12</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="20"/>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E18" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E19" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E20" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E17" s="9" t="s">
+    <row r="21" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E21" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E18" s="9" t="s">
+    <row r="22" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E22" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E19" s="9" t="s">
+    <row r="23" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E23" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E20" s="10" t="s">
+    <row r="24" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E24" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E21" s="10" t="s">
+    <row r="25" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E25" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E22" s="10" t="s">
+    <row r="26" spans="5:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E26" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E23" s="10" t="s">
+    <row r="27" spans="5:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="9" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E24" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E25" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E26" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E27" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HP updated weekly material
</commit_message>
<xml_diff>
--- a/CourseStructrure_AY2023-24.xlsx
+++ b/CourseStructrure_AY2023-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/hp12384_bristol_ac_uk/Documents/Teaching/UoB/EMAT10007_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{94D3B256-24FF-4E4F-8D7C-06948EE92458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D7434F7-070F-D145-9855-37B91F6CA1C2}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{94D3B256-24FF-4E4F-8D7C-06948EE92458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC18EF1B-DFFC-6541-AD8E-D636EA877C87}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{EB69D0A4-597B-4DBB-A11D-3E8D6AA8DFB6}"/>
   </bookViews>
@@ -59,30 +59,18 @@
     <t>Programming Fundamentals</t>
   </si>
   <si>
-    <t>Data Structures (Lists)</t>
-  </si>
-  <si>
     <t>Working with data</t>
   </si>
   <si>
     <t>Writing code that works</t>
   </si>
   <si>
-    <t>Functions 2 (scope)</t>
-  </si>
-  <si>
-    <t>Functions 1 (define, returning)</t>
-  </si>
-  <si>
     <t>Algorithms and the notional machine</t>
   </si>
   <si>
     <t>Teach yourself</t>
   </si>
   <si>
-    <t>Consolidation 2 - descriptive statistics of a data set (w/ independent use of a python module for statistical analysis)</t>
-  </si>
-  <si>
     <t>Decomposition</t>
   </si>
   <si>
@@ -125,12 +113,6 @@
     <t>Week 12: Going further with programming &amp; optional coursework support session (MH)</t>
   </si>
   <si>
-    <t>Consolidation 3 - Refactoring and extending code -&gt; Testing and ChatGPT</t>
-  </si>
-  <si>
-    <t>Consolidation 1 - Turtlesim? Text-based adventure game? + debugging</t>
-  </si>
-  <si>
     <t>Final CW submission</t>
   </si>
   <si>
@@ -140,22 +122,40 @@
     <t>2022/23 structure for reference</t>
   </si>
   <si>
-    <t xml:space="preserve">Coursework support session </t>
-  </si>
-  <si>
-    <t>Objects, Variables &amp; Operators</t>
-  </si>
-  <si>
-    <t>Control Structures: Conditional Statements</t>
-  </si>
-  <si>
-    <t>Control Structures: Loops</t>
-  </si>
-  <si>
-    <t>Reading and plotting data, Matplotlib</t>
-  </si>
-  <si>
     <t>CW set</t>
+  </si>
+  <si>
+    <t>Objects, Variables &amp; Operators -- HP</t>
+  </si>
+  <si>
+    <t>Control Structures: Conditional Statements -- HP</t>
+  </si>
+  <si>
+    <t>Control Structures: Loops -- HP</t>
+  </si>
+  <si>
+    <t>Consolidation 1 - Turtlesim? Text-based adventure game? + debugging -- HP</t>
+  </si>
+  <si>
+    <t>Data Structures (Lists) -- MH</t>
+  </si>
+  <si>
+    <t>Functions 1 (define, returning) -- MH</t>
+  </si>
+  <si>
+    <t>Reading and plotting data, Matplotlib - MH</t>
+  </si>
+  <si>
+    <t>Consolidation 2 - descriptive statistics of a data set (w/ independent use of a python module for statistical analysis) - MH</t>
+  </si>
+  <si>
+    <t>Functions 2 (scope) -- MH</t>
+  </si>
+  <si>
+    <t>Coursework support session  - HP + MH</t>
+  </si>
+  <si>
+    <t>Consolidation 3 - Refactoring and extending code -&gt; Testing and ChatGPT - HP</t>
   </si>
 </sst>
 </file>
@@ -367,6 +367,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -378,9 +381,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -399,6 +399,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -701,7 +705,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -731,21 +735,21 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="13"/>
@@ -754,10 +758,10 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="13"/>
@@ -766,10 +770,10 @@
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="13"/>
@@ -778,10 +782,10 @@
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="13"/>
@@ -790,10 +794,10 @@
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="13"/>
@@ -814,14 +818,14 @@
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>8</v>
+      <c r="C9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="13"/>
@@ -830,13 +834,13 @@
       <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G10" s="13"/>
     </row>
@@ -844,13 +848,13 @@
       <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="5" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G11" s="13"/>
     </row>
@@ -858,14 +862,14 @@
       <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>9</v>
+      <c r="C12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="13"/>
@@ -874,13 +878,13 @@
       <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="19"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G13" s="13"/>
     </row>
@@ -888,10 +892,10 @@
       <c r="B14" s="15">
         <v>12</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="15" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="13"/>
@@ -899,65 +903,65 @@
     <row r="15" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E17" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E18" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E19" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E20" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E21" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E22" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E23" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E24" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E25" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="5:5" ht="17" x14ac:dyDescent="0.2">
       <c r="E26" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="5:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E27" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>